<commit_message>
POI library added for reading Excel and code cleanup done. Also test case updated
</commit_message>
<xml_diff>
--- a/EbayAppAutomation/app/src/test/assets/EbayTestData.xlsx
+++ b/EbayAppAutomation/app/src/test/assets/EbayTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20140" yWindow="4820" windowWidth="24960" windowHeight="17960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Smile You Can Read Me !" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <t>rubanb.tech@gmail.com</t>
   </si>
   <si>
-    <t>HTCdesireHD&amp;2243</t>
+    <t>xxxxx</t>
   </si>
 </sst>
 </file>
@@ -349,55 +349,55 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.616494476084344</c:v>
+                  <c:v>0.121771825662088</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.385670011583382</c:v>
+                  <c:v>0.562775893753932</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.643686262598384</c:v>
+                  <c:v>0.482271486327466</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.560956725141149</c:v>
+                  <c:v>0.862655115029024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.122969939657859</c:v>
+                  <c:v>0.646861408280683</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.825071194383406</c:v>
+                  <c:v>0.911818167624852</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51223678458653</c:v>
+                  <c:v>0.963315726515915</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.526985919330223</c:v>
+                  <c:v>0.703240209442515</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.000814434013461706</c:v>
+                  <c:v>0.206517319723696</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.162461559607187</c:v>
+                  <c:v>0.288401315204771</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.723523544373032</c:v>
+                  <c:v>0.73659048043703</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.207315915247319</c:v>
+                  <c:v>0.730984752638442</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.503635826782199</c:v>
+                  <c:v>0.867861144807937</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.85912999895259</c:v>
+                  <c:v>0.234018394073919</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.624531238086963</c:v>
+                  <c:v>0.562276408650263</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.314775870416399</c:v>
+                  <c:v>0.325321780982361</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0251518286221928</c:v>
+                  <c:v>0.262711801881689</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -409,55 +409,55 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.730424605979275</c:v>
+                  <c:v>0.377412918985662</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0968453067843309</c:v>
+                  <c:v>0.94437231574624</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.529902520819638</c:v>
+                  <c:v>0.0165219835498099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.213190735453703</c:v>
+                  <c:v>0.16193643384637</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.150053305283561</c:v>
+                  <c:v>0.900134284615284</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.395934651871662</c:v>
+                  <c:v>0.199173979068444</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.85462112395605</c:v>
+                  <c:v>0.50582028438603</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.380720263166043</c:v>
+                  <c:v>0.304866333205761</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.927735625716377</c:v>
+                  <c:v>0.110437348358814</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.171555260200451</c:v>
+                  <c:v>0.359429474867064</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.529546418950965</c:v>
+                  <c:v>0.942786335645973</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.427249573913816</c:v>
+                  <c:v>0.189439926585355</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.383448036459539</c:v>
+                  <c:v>0.111176497043225</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.361087457326769</c:v>
+                  <c:v>0.778498854440014</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0864177539575374</c:v>
+                  <c:v>0.762120446419852</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.257918775092239</c:v>
+                  <c:v>0.956261813672804</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.738566678380673</c:v>
+                  <c:v>0.128486043322192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -472,11 +472,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2119517624"/>
-        <c:axId val="2119528312"/>
+        <c:axId val="2119849128"/>
+        <c:axId val="2119863752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2119517624"/>
+        <c:axId val="2119849128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -561,12 +561,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119528312"/>
+        <c:crossAx val="2119863752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2119528312"/>
+        <c:axId val="2119863752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -651,7 +651,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119517624"/>
+        <c:crossAx val="2119849128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -1275,171 +1275,171 @@
     <row r="7" spans="4:5">
       <c r="D7" s="1">
         <f ca="1">RAND()</f>
-        <v>0.61649447608434371</v>
+        <v>0.12177182566208788</v>
       </c>
       <c r="E7" s="1">
         <f ca="1">RAND()</f>
-        <v>0.73042460597927528</v>
+        <v>0.37741291898566243</v>
       </c>
     </row>
     <row r="8" spans="4:5">
       <c r="D8" s="1">
         <f t="shared" ref="D8:E23" ca="1" si="0">RAND()</f>
-        <v>0.38567001158338243</v>
+        <v>0.56277589375393244</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6845306784330898E-2</v>
+        <v>0.94437231574624037</v>
       </c>
     </row>
     <row r="9" spans="4:5">
       <c r="D9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64368626259838446</v>
+        <v>0.4822714863274663</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52990252081963762</v>
+        <v>1.6521983549809938E-2</v>
       </c>
     </row>
     <row r="10" spans="4:5">
       <c r="D10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56095672514114858</v>
+        <v>0.86265511502902381</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21319073545370326</v>
+        <v>0.16193643384637002</v>
       </c>
     </row>
     <row r="11" spans="4:5">
       <c r="D11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12296993965785941</v>
+        <v>0.6468614082806835</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15005330528356109</v>
+        <v>0.90013428461528422</v>
       </c>
     </row>
     <row r="12" spans="4:5">
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82507119438340559</v>
+        <v>0.91181816762485202</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39593465187166188</v>
+        <v>0.19917397906844403</v>
       </c>
     </row>
     <row r="13" spans="4:5">
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51223678458653032</v>
+        <v>0.96331572651591491</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85462112395605039</v>
+        <v>0.50582028438603011</v>
       </c>
     </row>
     <row r="14" spans="4:5">
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52698591933022276</v>
+        <v>0.70324020944251531</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38072026316604346</v>
+        <v>0.30486633320576062</v>
       </c>
     </row>
     <row r="15" spans="4:5">
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8.1443401346170674E-4</v>
+        <v>0.20651731972369569</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92773562571637747</v>
+        <v>0.11043734835881425</v>
       </c>
     </row>
     <row r="16" spans="4:5">
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16246155960718656</v>
+        <v>0.28840131520477141</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17155526020045109</v>
+        <v>0.359429474867064</v>
       </c>
     </row>
     <row r="17" spans="4:5">
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72352354437303212</v>
+        <v>0.73659048043703013</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52954641895096488</v>
+        <v>0.9427863356459727</v>
       </c>
     </row>
     <row r="18" spans="4:5">
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20731591524731929</v>
+        <v>0.73098475263844209</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42724957391381646</v>
+        <v>0.18943992658535547</v>
       </c>
     </row>
     <row r="19" spans="4:5">
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50363582678219865</v>
+        <v>0.86786114480793708</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38344803645953862</v>
+        <v>0.11117649704322485</v>
       </c>
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85912999895259001</v>
+        <v>0.23401839407391878</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36108745732676883</v>
+        <v>0.7784988544400141</v>
       </c>
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62453123808696265</v>
+        <v>0.56227640865026274</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6417753957537369E-2</v>
+        <v>0.76212044641985255</v>
       </c>
     </row>
     <row r="22" spans="4:5">
       <c r="D22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31477587041639921</v>
+        <v>0.3253217809823612</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25791877509223948</v>
+        <v>0.95626181367280394</v>
       </c>
     </row>
     <row r="23" spans="4:5">
       <c r="D23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5151828622192784E-2</v>
+        <v>0.26271180188168863</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73856667838067258</v>
+        <v>0.12848604332219193</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1464,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>